<commit_message>
Modified thesis work plan
</commit_message>
<xml_diff>
--- a/workbooks/thesis_work_plan.xlsx
+++ b/workbooks/thesis_work_plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Study of AOM and inherent patterns</t>
   </si>
@@ -41,6 +41,9 @@
   <si>
     <t>January 31</t>
   </si>
+  <si>
+    <t>Mining of Web Patterns for AOMs</t>
+  </si>
 </sst>
 </file>
 
@@ -55,7 +58,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +95,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCDE28"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -321,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -417,6 +426,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -425,6 +440,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFCDE28"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -713,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -874,25 +894,25 @@
     </row>
     <row r="6" spans="2:23">
       <c r="B6" s="26" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
       <c r="T6" s="15"/>
       <c r="U6" s="15"/>
       <c r="V6" s="15"/>
@@ -900,81 +920,107 @@
     </row>
     <row r="7" spans="2:23">
       <c r="B7" s="26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
       <c r="V7" s="15"/>
       <c r="W7" s="5"/>
     </row>
-    <row r="8" spans="2:23" ht="15.75" thickBot="1">
-      <c r="B8" s="27" t="s">
+    <row r="8" spans="2:23">
+      <c r="B8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="5"/>
+    </row>
+    <row r="9" spans="2:23" ht="15.75" thickBot="1">
+      <c r="B9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="6"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="6"/>
     </row>
-    <row r="9" spans="2:23" ht="70.5">
-      <c r="B9" s="28"/>
-      <c r="C9" s="7" t="s">
+    <row r="10" spans="2:23" ht="70.5">
+      <c r="B10" s="28"/>
+      <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="7" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="7" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated presentation and work plan
</commit_message>
<xml_diff>
--- a/workbooks/thesis_work_plan.xlsx
+++ b/workbooks/thesis_work_plan.xlsx
@@ -30,9 +30,6 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>Dissertation writing</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>Mining of Web Patterns for AOMs</t>
+  </si>
+  <si>
+    <t>Tests &amp; Validation</t>
   </si>
 </sst>
 </file>
@@ -419,6 +419,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -426,12 +432,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -736,7 +736,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -750,29 +750,29 @@
     <row r="1" spans="2:23" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:23" ht="15.75" thickBot="1">
       <c r="B2" s="26"/>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="34"/>
     </row>
     <row r="3" spans="2:23" ht="15.75" thickBot="1">
       <c r="B3" s="27"/>
@@ -894,14 +894,14 @@
     </row>
     <row r="6" spans="2:23">
       <c r="B6" s="26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -946,7 +946,7 @@
     </row>
     <row r="8" spans="2:23">
       <c r="B8" s="26" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="15"/>
@@ -972,7 +972,7 @@
     </row>
     <row r="9" spans="2:23" ht="15.75" thickBot="1">
       <c r="B9" s="27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="16"/>
@@ -999,7 +999,7 @@
     <row r="10" spans="2:23" ht="70.5">
       <c r="B10" s="28"/>
       <c r="C10" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1021,7 +1021,7 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>